<commit_message>
Thêm giao diện hệ thống gọi số và chỉnh sửa tính năng cập nhật thông tin cán bộ
Thêm giao diện hệ thống gọi số và chỉnh sửa tính năng cập nhật thông tin cán bộ
</commit_message>
<xml_diff>
--- a/WebServerAPI/WebServerAPI/Files/Book1.xlsx
+++ b/WebServerAPI/WebServerAPI/Files/Book1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuvi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D29809EA-F905-4C32-90E4-54D011380DCF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{19E5AB6C-7A12-4A50-B4C0-F3679C291459}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>Mã cán bộ</t>
+  </si>
   <si>
     <t>Họ tên</t>
   </si>
@@ -36,22 +38,31 @@
     <t>Tên bộ phận</t>
   </si>
   <si>
-    <t>Nguyễn Phú L</t>
-  </si>
-  <si>
-    <t>C:\Users\luuvi\Downloads\gopy.png</t>
-  </si>
-  <si>
-    <t>Nguyễn Tuấn M</t>
-  </si>
-  <si>
-    <t>Lĩnh vực tài nguyên và đất đai</t>
+    <t>cb14</t>
+  </si>
+  <si>
+    <t>Trần Quốc K</t>
+  </si>
+  <si>
+    <t>D:\meme.png</t>
+  </si>
+  <si>
+    <t>Lĩnh vực lao động, thương binh và xã hội</t>
+  </si>
+  <si>
+    <t>cb15</t>
+  </si>
+  <si>
+    <t>Trần Trung P</t>
+  </si>
+  <si>
+    <t>Lĩnh vực lao động, Thương Binh Và Xã Hội</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +128,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -129,7 +140,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -176,23 +187,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -228,23 +222,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -396,16 +373,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55135A7-5D04-4B7E-AAF2-D1B387890E63}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,27 +392,36 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chỉnh sửa thông báo cập nhật thông tin
Hoàn thành
</commit_message>
<xml_diff>
--- a/WebServerAPI/WebServerAPI/Files/Book1.xlsx
+++ b/WebServerAPI/WebServerAPI/Files/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,37 +26,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
+    <t>Hình ảnh</t>
+  </si>
+  <si>
     <t>Mã cán bộ</t>
   </si>
   <si>
     <t>Họ tên</t>
   </si>
   <si>
-    <t>Hình ảnh</t>
-  </si>
-  <si>
     <t>Tên bộ phận</t>
   </si>
   <si>
-    <t>cb14</t>
-  </si>
-  <si>
-    <t>Trần Quốc K</t>
-  </si>
-  <si>
-    <t>D:\meme.png</t>
-  </si>
-  <si>
-    <t>Lĩnh vực lao động, thương binh và xã hội</t>
-  </si>
-  <si>
-    <t>cb15</t>
-  </si>
-  <si>
-    <t>Trần Trung P</t>
-  </si>
-  <si>
-    <t>Lĩnh vực lao động, Thương Binh Và Xã Hội</t>
+    <t>cb43</t>
+  </si>
+  <si>
+    <t>Trần Quốc T</t>
+  </si>
+  <si>
+    <t>Lĩnh vực tài nguyên và đất đai</t>
+  </si>
+  <si>
+    <t>cb44</t>
+  </si>
+  <si>
+    <t>Hà Anh T</t>
+  </si>
+  <si>
+    <t>Lĩnh vực xây dựng</t>
+  </si>
+  <si>
+    <t>D:\images\user.png</t>
   </si>
 </sst>
 </file>
@@ -377,12 +377,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,35 +396,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>